<commit_message>
Fix for generating corrupted yaml when importing from excel using the mustBe and mustBeNot expectations.
</commit_message>
<xml_diff>
--- a/tests/fixtures/excel/shipments-odcs.xlsx
+++ b/tests/fixtures/excel/shipments-odcs.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jochen/Projects/open-data-contract-standard-excel-template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\datacontract-cli\tests\fixtures\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58ECC940-E1E1-584B-B311-B4AA053E9340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122725B7-598C-4FA6-BED9-424077697850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="1"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="8" r:id="rId1"/>
     <sheet name="Fundamentals" sheetId="10" r:id="rId2"/>
-    <sheet name="Schema shipments" r:id="rId16" sheetId="22"/>
+    <sheet name="Schema shipments" sheetId="22" r:id="rId3"/>
     <sheet name="Quality" sheetId="21" r:id="rId4"/>
     <sheet name="Support" sheetId="12" r:id="rId5"/>
     <sheet name="Team" sheetId="13" r:id="rId6"/>
@@ -44,6 +44,14 @@
     <definedName name="price.priceUnit">Pricing!$B$6</definedName>
     <definedName name="quality">Quality!$A$4:$AZ$300</definedName>
     <definedName name="roles" localSheetId="6">Roles!$A$4:$E$1000</definedName>
+    <definedName name="schema.businessName" localSheetId="2">'Schema shipments'!$B$8</definedName>
+    <definedName name="schema.dataGranularityDescription" localSheetId="2">'Schema shipments'!$B$10</definedName>
+    <definedName name="schema.description" localSheetId="2">'Schema shipments'!$B$7</definedName>
+    <definedName name="schema.name" localSheetId="2">'Schema shipments'!$B$5</definedName>
+    <definedName name="schema.physicalName" localSheetId="2">'Schema shipments'!$B$9</definedName>
+    <definedName name="schema.physicalType" localSheetId="2">'Schema shipments'!$B$6</definedName>
+    <definedName name="schema.properties" localSheetId="2">'Schema shipments'!$A$13:$L$981</definedName>
+    <definedName name="schema.tags" localSheetId="2">'Schema shipments'!$B$11</definedName>
     <definedName name="servers.azure.delimiter">Servers!$C$14</definedName>
     <definedName name="servers.azure.format">Servers!$C$13</definedName>
     <definedName name="servers.azure.location">Servers!$C$12</definedName>
@@ -107,16 +115,8 @@
     <definedName name="team">Team!$A$4:$G$1000</definedName>
     <definedName name="tenant">Fundamentals!$C$16</definedName>
     <definedName name="version">Fundamentals!$C$9</definedName>
-    <definedName name="schema.businessName" localSheetId="2">'Schema shipments'!$B$8</definedName>
-    <definedName name="schema.dataGranularityDescription" localSheetId="2">'Schema shipments'!$B$10</definedName>
-    <definedName name="schema.description" localSheetId="2">'Schema shipments'!$B$7</definedName>
-    <definedName name="schema.name" localSheetId="2">'Schema shipments'!$B$5</definedName>
-    <definedName name="schema.physicalName" localSheetId="2">'Schema shipments'!$B$9</definedName>
-    <definedName name="schema.physicalType" localSheetId="2">'Schema shipments'!$B$6</definedName>
-    <definedName name="schema.properties" localSheetId="2">'Schema shipments'!$A$13:$L$981</definedName>
-    <definedName name="schema.tags" localSheetId="2">'Schema shipments'!$B$11</definedName>
   </definedNames>
-  <calcPr calcId="191029" fullCalcOnLoad="true"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="267">
   <si>
     <t>Property</t>
   </si>
@@ -154,9 +154,6 @@
     <t>apiVersion</t>
   </si>
   <si>
-    <t>v3.0.2</t>
-  </si>
-  <si>
     <t>Logical Type</t>
   </si>
   <si>
@@ -290,9 +287,6 @@
   </si>
   <si>
     <t>Copy this sheet for every model in your data contract.</t>
-  </si>
-  <si>
-    <t>&lt;table_name&gt;</t>
   </si>
   <si>
     <t>Physical Name</t>
@@ -647,9 +641,6 @@
     <t>Shipments</t>
   </si>
   <si>
-    <t>1.0.1</t>
-  </si>
-  <si>
     <t>draft</t>
   </si>
   <si>
@@ -857,90 +848,107 @@
     <t>sql</t>
   </si>
   <si>
+    <t>SELECT COUNT(*) FROM shipments</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>additionalField</t>
+  </si>
+  <si>
+    <t>We added an addition field - b</t>
+  </si>
+  <si>
+    <t>slackname</t>
+  </si>
+  <si>
+    <t>http://find.me.here</t>
+  </si>
+  <si>
+    <t>slack</t>
+  </si>
+  <si>
+    <t>interactive</t>
+  </si>
+  <si>
+    <t>vimportant</t>
+  </si>
+  <si>
+    <t>administrator</t>
+  </si>
+  <si>
+    <t>2020-01-01</t>
+  </si>
+  <si>
+    <t>nimportant</t>
+  </si>
+  <si>
+    <t>reader</t>
+  </si>
+  <si>
+    <t>2024-10-10</t>
+  </si>
+  <si>
+    <t>availability</t>
+  </si>
+  <si>
+    <t>95%</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>operational</t>
+  </si>
+  <si>
+    <t>production</t>
+  </si>
+  <si>
+    <t>bigquery</t>
+  </si>
+  <si>
+    <t>acme_shipments_prod</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>Per 1000 requests</t>
+  </si>
+  <si>
+    <t>mustBe</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>confirming that the total number of records divided by 2 is 3.5</t>
+  </si>
+  <si>
+    <t>confirming that the total number of records  is 7</t>
+  </si>
+  <si>
+    <t>1.0.2</t>
+  </si>
+  <si>
+    <t>SELECT AVG(duration) FROM shipments</t>
+  </si>
+  <si>
     <t>Table shall contain at least 1 row</t>
   </si>
   <si>
-    <t>SELECT COUNT(*) FROM shipments</t>
-  </si>
-  <si>
     <t>mustBeGreaterThanOrEqualTo</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>{field} must contain the field "destination"</t>
-  </si>
-  <si>
-    <t>additionalField</t>
-  </si>
-  <si>
-    <t>We added an addition field - b</t>
-  </si>
-  <si>
-    <t>slackname</t>
-  </si>
-  <si>
-    <t>http://find.me.here</t>
-  </si>
-  <si>
-    <t>slack</t>
-  </si>
-  <si>
-    <t>interactive</t>
-  </si>
-  <si>
-    <t>vimportant</t>
-  </si>
-  <si>
-    <t>administrator</t>
-  </si>
-  <si>
-    <t>2020-01-01</t>
-  </si>
-  <si>
-    <t>nimportant</t>
-  </si>
-  <si>
-    <t>reader</t>
-  </si>
-  <si>
-    <t>2024-10-10</t>
-  </si>
-  <si>
-    <t>availability</t>
-  </si>
-  <si>
-    <t>95%</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>operational</t>
-  </si>
-  <si>
-    <t>production</t>
-  </si>
-  <si>
-    <t>bigquery</t>
-  </si>
-  <si>
-    <t>acme_shipments_prod</t>
-  </si>
-  <si>
-    <t>EUR</t>
-  </si>
-  <si>
-    <t>Per 1000 requests</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -990,6 +998,25 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Mono"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1153,7 +1180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1223,6 +1250,39 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1240,21 +1300,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1639,42 +1684,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView topLeftCell="A9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="14.0"/>
-    <col min="2" max="16384" style="3" width="8.83203125"/>
+    <col min="1" max="1" width="14" style="3" customWidth="1"/>
+    <col min="2" max="16384" width="8.796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A2" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A7" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -1685,9 +1730,9 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A8" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -1698,9 +1743,9 @@
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A9" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -1711,9 +1756,9 @@
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
     </row>
-    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A10" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
@@ -1724,9 +1769,9 @@
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A11" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
@@ -1737,7 +1782,7 @@
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
@@ -1748,7 +1793,7 @@
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
     </row>
-    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -1759,9 +1804,9 @@
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A14" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -1772,9 +1817,9 @@
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A15" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -1785,9 +1830,9 @@
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A16" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
@@ -1798,9 +1843,9 @@
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
     </row>
-    <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A17" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
@@ -1811,12 +1856,12 @@
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
     </row>
-    <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A18" s="23" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
@@ -1826,10 +1871,10 @@
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
     </row>
-    <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A19" s="23"/>
       <c r="B19" s="24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
@@ -1839,7 +1884,7 @@
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
     </row>
-    <row r="20" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A20" s="13"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
@@ -1850,12 +1895,12 @@
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
     </row>
-    <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A21" s="25" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
@@ -1865,10 +1910,10 @@
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
     </row>
-    <row r="22" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A22" s="25"/>
       <c r="B22" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
@@ -1878,10 +1923,10 @@
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
     </row>
-    <row r="23" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A23" s="13"/>
       <c r="B23" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
@@ -1891,10 +1936,10 @@
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
     </row>
-    <row r="24" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A24" s="13"/>
       <c r="B24" s="13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
@@ -1904,7 +1949,7 @@
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
     </row>
-    <row r="25" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
@@ -1915,12 +1960,12 @@
       <c r="H25" s="13"/>
       <c r="I25" s="13"/>
     </row>
-    <row r="26" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A26" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="13" t="s">
         <v>40</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>41</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
@@ -1930,12 +1975,12 @@
       <c r="H26" s="13"/>
       <c r="I26" s="13"/>
     </row>
-    <row r="27" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A27" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
@@ -1945,12 +1990,12 @@
       <c r="H27" s="13"/>
       <c r="I27" s="13"/>
     </row>
-    <row r="28" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A28" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="13" t="s">
         <v>42</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>43</v>
       </c>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
@@ -1960,7 +2005,7 @@
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
@@ -1971,7 +2016,7 @@
       <c r="H29" s="13"/>
       <c r="I29" s="13"/>
     </row>
-    <row r="30" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
@@ -1982,7 +2027,7 @@
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
     </row>
-    <row r="31" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -1995,10 +2040,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B24" r:id="rId2"/>
+    <hyperlink ref="B24" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2008,46 +2053,46 @@
   <sheetViews>
     <sheetView zoomScale="165" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="22" width="26.1640625"/>
-    <col min="2" max="2" customWidth="true" style="22" width="22.33203125"/>
-    <col min="3" max="16384" style="22" width="10.83203125"/>
+    <col min="1" max="1" width="26.1328125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="22" customWidth="1"/>
+    <col min="3" max="16384" width="10.796875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="2" customFormat="1" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A2" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.5"/>
+    <row r="4" spans="1:2" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A4" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A5" s="7" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:2" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="B5" s="5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A6" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>94</v>
-      </c>
       <c r="B6" s="5" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -2068,24 +2113,24 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="33.1640625"/>
-    <col min="2" max="2" customWidth="true" style="2" width="90.0"/>
-    <col min="3" max="16384" style="2" width="8.83203125"/>
+    <col min="1" max="1" width="33.1328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="90" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A2" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
@@ -2093,80 +2138,80 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A5" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="5" t="str">
         <f>IF(owner&lt;&gt;"",owner,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>fulfillment</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A6" s="5" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
     </row>
@@ -2183,184 +2228,184 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="2.83203125"/>
-    <col min="2" max="2" customWidth="true" style="2" width="19.6640625"/>
-    <col min="3" max="3" customWidth="true" style="2" width="45.0"/>
-    <col min="4" max="4" customWidth="true" style="2" width="1.83203125"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="28.1640625"/>
-    <col min="6" max="6" customWidth="true" style="2" width="14.33203125"/>
-    <col min="7" max="8" customWidth="true" style="2" width="10.0"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="14.1640625"/>
-    <col min="10" max="11" customWidth="true" style="2" width="14.33203125"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="23.5"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="24.1640625"/>
-    <col min="14" max="16384" style="2" width="8.83203125"/>
+    <col min="1" max="1" width="2.796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="45" style="2" customWidth="1"/>
+    <col min="4" max="4" width="1.796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="2" customWidth="1"/>
+    <col min="7" max="8" width="10" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="14.33203125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="23.46484375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A2" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A4" s="7" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A7" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A8" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="34" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A10" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="30"/>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A12" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="41"/>
       <c r="C12" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A14" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="5"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A15" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="5"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A16" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A18" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="7"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A19" s="7"/>
       <c r="B19" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A20" s="7"/>
       <c r="B20" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A21" s="7"/>
       <c r="B21" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A23" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -2382,131 +2427,133 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AL49"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="100" workbookViewId="0" tabSelected="false"/>
+    <sheetView zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:E5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="34.83203125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="24.0"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.5"/>
-    <col min="4" max="4" customWidth="true" style="2" width="17.5"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="8" width="28.1640625"/>
-    <col min="6" max="6" customWidth="true" style="2" width="35.6640625"/>
-    <col min="7" max="8" customWidth="true" style="2" width="10.0"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="14.1640625"/>
-    <col min="10" max="10" customWidth="true" style="2" width="14.33203125"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="28.1640625"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="28.6640625"/>
-    <col min="13" max="13" customWidth="true" style="2" width="28.6640625"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="11.6640625"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="19.0"/>
-    <col min="16" max="20" customWidth="true" style="2" width="19.0"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="2" width="21.6640625"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="2" width="27.33203125"/>
-    <col min="23" max="37" customWidth="true" style="2" width="15.5"/>
-    <col min="38" max="38" customWidth="true" style="2" width="26.1640625"/>
-    <col min="39" max="16384" style="2" width="8.83203125"/>
+    <col min="1" max="1" width="34.796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.46484375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.46484375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.1328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" style="2" customWidth="1"/>
+    <col min="7" max="8" width="10" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="28.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.6640625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="20" width="19" style="2" customWidth="1"/>
+    <col min="21" max="21" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="37" width="15.46484375" style="2" customWidth="1"/>
+    <col min="38" max="38" width="26.1328125" style="2" customWidth="1"/>
+    <col min="39" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.5">
+      <c r="A2" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.5">
+      <c r="A3" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.5">
+      <c r="A5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.5">
+      <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>176</v>
-      </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-    </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-    </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="B6" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="31" t="s">
-        <v>179</v>
-      </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-    </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="B7" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="34"/>
-    </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="B8" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="45"/>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A9" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="45"/>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.5">
+      <c r="A10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="45"/>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.5">
+      <c r="A11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="42" t="s">
         <v>177</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="34"/>
-    </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>178</v>
-      </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="34"/>
-    </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>180</v>
-      </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-    </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.5">
       <c r="W12" s="19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="X12" s="20"/>
       <c r="Y12" s="20"/>
@@ -2523,21 +2570,21 @@
       <c r="AJ12" s="20"/>
       <c r="AK12" s="21"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A13" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>10</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>11</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>3</v>
@@ -2546,117 +2593,117 @@
         <v>2</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="K13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="K13" s="10" t="s">
+      <c r="L13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="L13" s="10" t="s">
-        <v>15</v>
-      </c>
       <c r="M13" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N13" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="O13" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="P13" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q13" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="O13" s="10" t="s">
+      <c r="R13" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="P13" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q13" s="10" t="s">
+      <c r="S13" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="R13" s="10" t="s">
+      <c r="T13" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="S13" s="10" t="s">
+      <c r="U13" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="T13" s="10" t="s">
+      <c r="V13" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="U13" s="10" t="s">
+      <c r="W13" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="V13" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="W13" s="10" t="s">
+      <c r="X13" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="X13" s="10" t="s">
+      <c r="Y13" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z13" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="Y13" s="10" t="s">
+      <c r="AA13" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB13" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC13" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="AD13" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE13" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="Z13" s="10" t="s">
+      <c r="AF13" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="AA13" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB13" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="AC13" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="AD13" s="10" t="s">
+      <c r="AG13" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH13" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="AI13" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="AE13" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="AF13" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="AG13" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="AH13" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="AI13" s="10" t="s">
+      <c r="AJ13" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="AK13" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="AJ13" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="AK13" s="10" t="s">
-        <v>89</v>
-      </c>
       <c r="AL13" s="10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A14" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="E14" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="F14" s="15" t="s">
         <v>183</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>186</v>
       </c>
       <c r="G14" s="15" t="b">
         <v>0</v>
@@ -2665,19 +2712,19 @@
         <v>0</v>
       </c>
       <c r="I14" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="L14" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="J14" s="15" t="s">
+      <c r="M14" s="15" t="s">
         <v>188</v>
-      </c>
-      <c r="K14" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="L14" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="M14" s="15" t="s">
-        <v>191</v>
       </c>
       <c r="N14" s="15" t="b">
         <v>1</v>
@@ -2711,14 +2758,14 @@
       <c r="AK14" s="15"/>
       <c r="AL14" s="28"/>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:38" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A15" s="17" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E15" s="16"/>
       <c r="F15" s="15"/>
@@ -2727,13 +2774,13 @@
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
       <c r="K15" s="15" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="L15" s="15" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="M15" s="15" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="N15" s="15" t="b">
         <v>0</v>
@@ -2765,24 +2812,24 @@
       <c r="AK15" s="15"/>
       <c r="AL15" s="28"/>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:38" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A16" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="D16" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="E16" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="F16" s="15" t="s">
         <v>198</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>201</v>
       </c>
       <c r="G16" s="15" t="b">
         <v>0</v>
@@ -2791,7 +2838,7 @@
         <v>0</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
@@ -2829,24 +2876,24 @@
       <c r="AK16" s="15"/>
       <c r="AL16" s="28"/>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:38" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A17" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="F17" s="15" t="s">
         <v>202</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>205</v>
       </c>
       <c r="G17" s="15" t="b">
         <v>0</v>
@@ -2855,7 +2902,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
@@ -2893,24 +2940,24 @@
       <c r="AK17" s="15"/>
       <c r="AL17" s="28"/>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:38" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A18" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="F18" s="15" t="s">
         <v>206</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>209</v>
       </c>
       <c r="G18" s="15" t="b">
         <v>0</v>
@@ -2919,7 +2966,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
@@ -2957,24 +3004,24 @@
       <c r="AK18" s="15"/>
       <c r="AL18" s="28"/>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A19" s="17" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G19" s="15" t="b">
         <v>0</v>
@@ -2983,7 +3030,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
@@ -3021,24 +3068,24 @@
       <c r="AK19" s="15"/>
       <c r="AL19" s="28"/>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:38" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A20" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="D20" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="E20" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="F20" s="15" t="s">
         <v>216</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>218</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>219</v>
       </c>
       <c r="G20" s="15" t="b">
         <v>0</v>
@@ -3047,7 +3094,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
@@ -3061,7 +3108,7 @@
         <v>0</v>
       </c>
       <c r="Q20" s="15" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="R20" s="15"/>
       <c r="S20" s="15"/>
@@ -3087,29 +3134,29 @@
       <c r="AK20" s="15"/>
       <c r="AL20" s="28"/>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A21" s="18" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E21" s="16"/>
       <c r="F21" s="15" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G21" s="15" t="b">
         <v>1</v>
       </c>
       <c r="H21" s="15"/>
       <c r="I21" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
@@ -3141,24 +3188,24 @@
       <c r="AK21" s="15"/>
       <c r="AL21" s="28"/>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A22" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="F22" s="15" t="s">
         <v>225</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>226</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>228</v>
       </c>
       <c r="G22" s="15" t="b">
         <v>1</v>
@@ -3167,7 +3214,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J22" s="15"/>
       <c r="K22" s="15"/>
@@ -3203,24 +3250,24 @@
       <c r="AK22" s="15"/>
       <c r="AL22" s="28"/>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A23" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="F23" s="15" t="s">
         <v>229</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>230</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>231</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>232</v>
       </c>
       <c r="G23" s="15" t="b">
         <v>1</v>
@@ -3229,7 +3276,7 @@
         <v>0</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J23" s="15"/>
       <c r="K23" s="15"/>
@@ -3265,31 +3312,31 @@
       <c r="AK23" s="15"/>
       <c r="AL23" s="28"/>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A24" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="F24" s="15" t="s">
         <v>233</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>234</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>235</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>236</v>
       </c>
       <c r="G24" s="15" t="b">
         <v>1</v>
       </c>
       <c r="H24" s="15"/>
       <c r="I24" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J24" s="15"/>
       <c r="K24" s="15"/>
@@ -3325,7 +3372,7 @@
       <c r="AK24" s="15"/>
       <c r="AL24" s="28"/>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A25" s="17"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
@@ -3365,7 +3412,7 @@
       <c r="AK25" s="15"/>
       <c r="AL25" s="28"/>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A26" s="17"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -3405,7 +3452,7 @@
       <c r="AK26" s="15"/>
       <c r="AL26" s="28"/>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A27" s="17"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
@@ -3445,7 +3492,7 @@
       <c r="AK27" s="15"/>
       <c r="AL27" s="28"/>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A28" s="17"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -3485,7 +3532,7 @@
       <c r="AK28" s="15"/>
       <c r="AL28" s="28"/>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A29" s="17"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -3525,7 +3572,7 @@
       <c r="AK29" s="15"/>
       <c r="AL29" s="28"/>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A30" s="17"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -3565,7 +3612,7 @@
       <c r="AK30" s="15"/>
       <c r="AL30" s="28"/>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A31" s="17"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -3605,7 +3652,7 @@
       <c r="AK31" s="15"/>
       <c r="AL31" s="28"/>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A32" s="17"/>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -3645,7 +3692,7 @@
       <c r="AK32" s="15"/>
       <c r="AL32" s="28"/>
     </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A33" s="17"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -3685,7 +3732,7 @@
       <c r="AK33" s="15"/>
       <c r="AL33" s="28"/>
     </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A34" s="17"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -3725,7 +3772,7 @@
       <c r="AK34" s="15"/>
       <c r="AL34" s="28"/>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A35" s="17"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -3765,7 +3812,7 @@
       <c r="AK35" s="15"/>
       <c r="AL35" s="28"/>
     </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A36" s="17"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
@@ -3805,7 +3852,7 @@
       <c r="AK36" s="15"/>
       <c r="AL36" s="28"/>
     </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A37" s="17"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -3845,7 +3892,7 @@
       <c r="AK37" s="15"/>
       <c r="AL37" s="28"/>
     </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A38" s="17"/>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
@@ -3885,7 +3932,7 @@
       <c r="AK38" s="15"/>
       <c r="AL38" s="28"/>
     </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A39" s="17"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -3925,7 +3972,7 @@
       <c r="AK39" s="15"/>
       <c r="AL39" s="28"/>
     </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A40" s="17"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
@@ -3965,7 +4012,7 @@
       <c r="AK40" s="15"/>
       <c r="AL40" s="28"/>
     </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A41" s="17"/>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
@@ -4005,7 +4052,7 @@
       <c r="AK41" s="15"/>
       <c r="AL41" s="28"/>
     </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A42" s="17"/>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
@@ -4045,7 +4092,7 @@
       <c r="AK42" s="15"/>
       <c r="AL42" s="28"/>
     </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A43" s="17"/>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
@@ -4085,7 +4132,7 @@
       <c r="AK43" s="15"/>
       <c r="AL43" s="28"/>
     </row>
-    <row r="44" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A44" s="17"/>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
@@ -4125,7 +4172,7 @@
       <c r="AK44" s="15"/>
       <c r="AL44" s="28"/>
     </row>
-    <row r="45" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A45" s="17"/>
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
@@ -4165,7 +4212,7 @@
       <c r="AK45" s="15"/>
       <c r="AL45" s="28"/>
     </row>
-    <row r="46" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A46" s="17"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
@@ -4205,7 +4252,7 @@
       <c r="AK46" s="15"/>
       <c r="AL46" s="28"/>
     </row>
-    <row r="47" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A47" s="17"/>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
@@ -4245,7 +4292,7 @@
       <c r="AK47" s="15"/>
       <c r="AL47" s="28"/>
     </row>
-    <row r="48" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A48" s="17"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -4285,7 +4332,7 @@
       <c r="AK48" s="15"/>
       <c r="AL48" s="28"/>
     </row>
-    <row r="49" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A49" s="17"/>
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
@@ -4368,105 +4415,105 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0F4C5A-BE41-6140-9B9B-80B8DB7D1AD7}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="36" width="17.5"/>
-    <col min="2" max="2" customWidth="true" style="36" width="22.0"/>
-    <col min="3" max="3" customWidth="true" style="36" width="14.33203125"/>
-    <col min="4" max="4" customWidth="true" style="36" width="32.6640625"/>
-    <col min="5" max="5" customWidth="true" style="36" width="18.33203125"/>
-    <col min="6" max="6" customWidth="true" style="36" width="28.33203125"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="36" width="19.0"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="36" width="16.0"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="36" width="22.83203125"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="36" width="23.5"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="36" width="15.5"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="36" width="17.83203125"/>
-    <col min="13" max="13" customWidth="true" style="36" width="17.83203125"/>
-    <col min="14" max="16384" style="36" width="8.83203125"/>
+    <col min="1" max="1" width="17.46484375" style="30" customWidth="1"/>
+    <col min="2" max="2" width="22" style="30" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="30" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" style="30" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" style="30" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" style="30" customWidth="1"/>
+    <col min="7" max="7" width="19" style="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" style="30" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.796875" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.46484375" style="30" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.46484375" style="30" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.796875" style="30" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.796875" style="30" customWidth="1"/>
+    <col min="14" max="16384" width="8.796875" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:13" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="A1" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" s="29"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A2" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="31"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A4" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="G4" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="35"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
+      <c r="H4" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="B2" s="37"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="39" t="s">
+      <c r="I4" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="J4" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="K4" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="L4" s="33" t="s">
         <v>159</v>
       </c>
-      <c r="F4" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="G4" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="H4" s="39" t="s">
-        <v>155</v>
-      </c>
-      <c r="I4" s="39" t="s">
-        <v>158</v>
-      </c>
-      <c r="J4" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="K4" s="39" t="s">
+      <c r="M4" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="L4" s="39" t="s">
-        <v>161</v>
-      </c>
-      <c r="M4" s="39" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="15" t="s">
-        <v>237</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>240</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>241</v>
+    </row>
+    <row r="5" spans="1:13" ht="31.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="38" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" s="38"/>
+      <c r="C5" s="37" t="s">
+        <v>234</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>264</v>
+      </c>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="G5" s="37" t="s">
+        <v>265</v>
+      </c>
+      <c r="H5" s="37" t="s">
+        <v>236</v>
       </c>
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
@@ -4474,64 +4521,88 @@
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
+    <row r="6" spans="1:13" ht="31.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="38" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>211</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>266</v>
+      </c>
+      <c r="E6" s="37"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
+    <row r="7" spans="1:13" ht="31.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="17" t="s">
+        <v>173</v>
+      </c>
       <c r="B7" s="17"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
+      <c r="C7" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>261</v>
+      </c>
       <c r="E7" s="15"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="17"/>
+      <c r="F7" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="H7" s="15">
+        <v>7</v>
+      </c>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+    </row>
+    <row r="8" spans="1:13" ht="31.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="17" t="s">
+        <v>173</v>
+      </c>
       <c r="B8" s="17"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
+      <c r="C8" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>260</v>
+      </c>
       <c r="E8" s="15"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F8" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
+      <c r="D9" s="17"/>
       <c r="E9" s="15"/>
       <c r="F9" s="27"/>
       <c r="G9" s="15"/>
@@ -4542,11 +4613,11 @@
       <c r="L9" s="15"/>
       <c r="M9" s="15"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
+      <c r="D10" s="17"/>
       <c r="E10" s="15"/>
       <c r="F10" s="27"/>
       <c r="G10" s="15"/>
@@ -4557,11 +4628,11 @@
       <c r="L10" s="15"/>
       <c r="M10" s="15"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="17"/>
       <c r="B11" s="17"/>
       <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
+      <c r="D11" s="17"/>
       <c r="E11" s="15"/>
       <c r="F11" s="27"/>
       <c r="G11" s="15"/>
@@ -4572,11 +4643,11 @@
       <c r="L11" s="15"/>
       <c r="M11" s="15"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
       <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
+      <c r="D12" s="17"/>
       <c r="E12" s="15"/>
       <c r="F12" s="27"/>
       <c r="G12" s="15"/>
@@ -4587,11 +4658,11 @@
       <c r="L12" s="15"/>
       <c r="M12" s="15"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
       <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
+      <c r="D13" s="17"/>
       <c r="E13" s="15"/>
       <c r="F13" s="27"/>
       <c r="G13" s="15"/>
@@ -4602,11 +4673,11 @@
       <c r="L13" s="15"/>
       <c r="M13" s="15"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="17"/>
       <c r="B14" s="17"/>
       <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
+      <c r="D14" s="17"/>
       <c r="E14" s="15"/>
       <c r="F14" s="27"/>
       <c r="G14" s="15"/>
@@ -4617,11 +4688,11 @@
       <c r="L14" s="15"/>
       <c r="M14" s="15"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="17"/>
       <c r="B15" s="17"/>
       <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
+      <c r="D15" s="17"/>
       <c r="E15" s="15"/>
       <c r="F15" s="27"/>
       <c r="G15" s="15"/>
@@ -4632,11 +4703,11 @@
       <c r="L15" s="15"/>
       <c r="M15" s="15"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
       <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
+      <c r="D16" s="17"/>
       <c r="E16" s="15"/>
       <c r="F16" s="27"/>
       <c r="G16" s="15"/>
@@ -4647,11 +4718,11 @@
       <c r="L16" s="15"/>
       <c r="M16" s="15"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
+      <c r="D17" s="17"/>
       <c r="E17" s="15"/>
       <c r="F17" s="27"/>
       <c r="G17" s="15"/>
@@ -4662,11 +4733,11 @@
       <c r="L17" s="15"/>
       <c r="M17" s="15"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
+      <c r="D18" s="17"/>
       <c r="E18" s="15"/>
       <c r="F18" s="27"/>
       <c r="G18" s="15"/>
@@ -4677,11 +4748,11 @@
       <c r="L18" s="15"/>
       <c r="M18" s="15"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="17"/>
       <c r="B19" s="17"/>
       <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
+      <c r="D19" s="17"/>
       <c r="E19" s="15"/>
       <c r="F19" s="27"/>
       <c r="G19" s="15"/>
@@ -4692,11 +4763,11 @@
       <c r="L19" s="15"/>
       <c r="M19" s="15"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="17"/>
       <c r="B20" s="17"/>
       <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
+      <c r="D20" s="17"/>
       <c r="E20" s="15"/>
       <c r="F20" s="27"/>
       <c r="G20" s="15"/>
@@ -4707,11 +4778,11 @@
       <c r="L20" s="15"/>
       <c r="M20" s="15"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="17"/>
       <c r="B21" s="17"/>
       <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
+      <c r="D21" s="17"/>
       <c r="E21" s="15"/>
       <c r="F21" s="27"/>
       <c r="G21" s="15"/>
@@ -4740,6 +4811,10 @@
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Severity" prompt="The severity of the data quality rule, such as error or warning." sqref="K5:K21" xr:uid="{0F4D661D-23D9-2540-B241-435A8E49610F}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Implementation" prompt="The data quality check in the engine's specific format." sqref="J5:J21" xr:uid="{00416CE8-FD1E-374C-B0CF-0FDCB1952802}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Engine" prompt="Required for custom DQ rule: name of the third-party engine being used. Any value is authorized here but common values are soda, greatExpectations, montecarlo, etc." sqref="I5:I21" xr:uid="{0459F568-8532-4048-9CA7-5708CD6DF179}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Schema" prompt="The schema name must match the name of the schema (table, ...) in the previous sheets." sqref="A4" xr:uid="{67CAE90D-676C-A44B-B965-361A399ACA9A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Property" prompt="Optional: Leave empty, if this is a schema-level quality check._x000a_The property must match the property name in the schema._x000a_" sqref="B4" xr:uid="{F3E67713-E117-6E46-AEFE-6861F5933838}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Rule" prompt="The predefined data quality rule from the library._x000a_Only appliable if &quot;Quality Type&quot; is set to &quot;library&quot; or empty (which is library by default, if a rule is defined)" sqref="E4" xr:uid="{4E8AA24F-1E70-FF4C-81CC-D9A25B05246C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality" prompt="The expected or guaranteed data quality from a business perspective._x000a__x000a_Maps to quality.description" sqref="D5:D21" xr:uid="{C84C6FF8-FC8D-B848-AC69-3DB82C6CB871}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Threshold Value" prompt="The acutal value for the treshold operator._x000a_For mustBeBetween adn mustNotBeBetween, use [lowerBoundry, upperBoundy] syntax, e.g. [0, 100]." sqref="H5:H21" xr:uid="{E792E24E-6B57-A948-A026-4637119AD944}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Quality Operator" prompt="The comparation operator specifies the condition to validate the rule._x000a_Use it together with the threshold value, e.g. mustBe 0, or mustBeBetween [0,100]_x000a_This is applicable for quality type sql and some library rules." sqref="G5:G21" xr:uid="{15B1EE74-8A6D-3F49-A7EC-55C27203D116}">
       <formula1>"mustBe, mustNotBe, mustBeGreaterThan, mustBeGreaterOrEqualTo, mustBeLessThan, mustBeLessOrEqualTo, mustBeBetween, mustNotBeBetween"</formula1>
@@ -4751,10 +4826,6 @@
     <dataValidation type="list" allowBlank="1" sqref="C5:C21" xr:uid="{664F88A2-7556-9B4E-A851-8889D6576B99}">
       <formula1>"text,library,sql,custom"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality" prompt="The expected or guaranteed data quality from a business perspective._x000a__x000a_Maps to quality.description" sqref="D5:D21" xr:uid="{C84C6FF8-FC8D-B848-AC69-3DB82C6CB871}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Schema" prompt="The schema name must match the name of the schema (table, ...) in the previous sheets." sqref="A4" xr:uid="{67CAE90D-676C-A44B-B965-361A399ACA9A}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Property" prompt="Optional: Leave empty, if this is a schema-level quality check._x000a_The property must match the property name in the schema._x000a_" sqref="B4" xr:uid="{F3E67713-E117-6E46-AEFE-6861F5933838}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Rule" prompt="The predefined data quality rule from the library._x000a_Only appliable if &quot;Quality Type&quot; is set to &quot;library&quot; or empty (which is library by default, if a rule is defined)" sqref="E4" xr:uid="{4E8AA24F-1E70-FF4C-81CC-D9A25B05246C}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4768,61 +4839,61 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="33.1640625"/>
-    <col min="2" max="3" customWidth="true" style="2" width="59.6640625"/>
-    <col min="4" max="6" customWidth="true" style="2" width="23.6640625"/>
-    <col min="7" max="16384" style="2" width="8.83203125"/>
+    <col min="1" max="1" width="33.1328125" style="2" customWidth="1"/>
+    <col min="2" max="3" width="59.6640625" style="2" customWidth="1"/>
+    <col min="4" max="6" width="23.6640625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E4" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5" s="5" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -4830,7 +4901,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -4838,7 +4909,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -4846,7 +4917,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -4854,7 +4925,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -4862,7 +4933,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -4870,7 +4941,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -4878,7 +4949,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -4886,7 +4957,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -4894,7 +4965,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -4902,7 +4973,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -4910,7 +4981,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -4918,7 +4989,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -4926,7 +4997,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -4934,7 +5005,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -4942,7 +5013,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -4966,80 +5037,80 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="33.1640625"/>
-    <col min="2" max="3" customWidth="true" style="2" width="59.6640625"/>
-    <col min="4" max="7" customWidth="true" style="2" width="23.6640625"/>
-    <col min="8" max="16384" style="2" width="8.83203125"/>
+    <col min="1" max="1" width="33.1328125" style="2" customWidth="1"/>
+    <col min="2" max="3" width="59.6640625" style="2" customWidth="1"/>
+    <col min="4" max="7" width="23.6640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A2" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A4" s="9" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
-        <v>64</v>
-      </c>
       <c r="B4" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="G4" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" s="5" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6" s="5" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -5048,7 +5119,7 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -5057,7 +5128,7 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -5066,7 +5137,7 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -5075,7 +5146,7 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -5084,7 +5155,7 @@
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -5093,7 +5164,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -5102,7 +5173,7 @@
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -5111,7 +5182,7 @@
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -5120,7 +5191,7 @@
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -5129,7 +5200,7 @@
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -5138,7 +5209,7 @@
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -5147,7 +5218,7 @@
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -5156,7 +5227,7 @@
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -5165,7 +5236,7 @@
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -5190,156 +5261,156 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="33.1640625"/>
-    <col min="2" max="2" customWidth="true" style="2" width="59.6640625"/>
-    <col min="3" max="3" customWidth="true" style="2" width="39.33203125"/>
-    <col min="4" max="4" customWidth="true" style="2" width="32.83203125"/>
-    <col min="5" max="5" customWidth="true" style="2" width="34.6640625"/>
-    <col min="6" max="16384" style="2" width="8.83203125"/>
+    <col min="1" max="1" width="33.1328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="59.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="39.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="32.796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="34.6640625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A2" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A4" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -5360,36 +5431,36 @@
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="33.1640625"/>
-    <col min="2" max="2" customWidth="true" style="2" width="59.6640625"/>
-    <col min="3" max="3" customWidth="true" style="2" width="39.33203125"/>
-    <col min="4" max="5" customWidth="true" style="2" width="32.83203125"/>
-    <col min="6" max="6" customWidth="true" style="2" width="34.6640625"/>
-    <col min="7" max="16384" style="2" width="8.83203125"/>
+    <col min="1" max="1" width="33.1328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="59.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="39.33203125" style="2" customWidth="1"/>
+    <col min="4" max="5" width="32.796875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="34.6640625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A2" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A4" s="7" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>103</v>
-      </c>
       <c r="B4" s="26"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" s="9" t="s">
         <v>0</v>
       </c>
@@ -5397,35 +5468,35 @@
         <v>1</v>
       </c>
       <c r="C6" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="F6" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7" s="5" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -5433,7 +5504,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -5441,7 +5512,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -5449,7 +5520,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -5457,7 +5528,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -5465,7 +5536,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -5473,7 +5544,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -5481,7 +5552,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -5489,7 +5560,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -5497,7 +5568,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -5505,7 +5576,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -5513,7 +5584,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -5521,7 +5592,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -5529,7 +5600,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -5537,7 +5608,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -5545,7 +5616,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -5568,54 +5639,54 @@
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="6.1640625"/>
-    <col min="2" max="2" customWidth="true" style="2" width="33.1640625"/>
-    <col min="3" max="6" customWidth="true" style="2" width="36.1640625"/>
-    <col min="7" max="22" customWidth="true" style="2" width="15.0"/>
-    <col min="23" max="30" customWidth="true" style="2" width="32.83203125"/>
-    <col min="31" max="31" customWidth="true" style="2" width="34.6640625"/>
-    <col min="32" max="16384" style="2" width="8.83203125"/>
+    <col min="1" max="1" width="6.1328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.1328125" style="2" customWidth="1"/>
+    <col min="3" max="6" width="36.1328125" style="2" customWidth="1"/>
+    <col min="7" max="22" width="15" style="2" customWidth="1"/>
+    <col min="23" max="30" width="32.796875" style="2" customWidth="1"/>
+    <col min="31" max="31" width="34.6640625" style="2" customWidth="1"/>
+    <col min="32" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A2" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="4"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A4" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B2" s="4"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>110</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
@@ -5625,607 +5696,607 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="5" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A12" s="7"/>
       <c r="B12" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A13" s="7"/>
       <c r="B13" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A14" s="7"/>
       <c r="B14" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A15" s="7"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A16" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A17" s="7"/>
       <c r="B17" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A18" s="7"/>
       <c r="B18" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A19" s="7"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A20" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A21" s="7"/>
       <c r="B21" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A22" s="7"/>
       <c r="B22" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A23" s="7"/>
       <c r="B23" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A24" s="7"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A25" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A26" s="7"/>
       <c r="B26" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A27" s="7"/>
       <c r="B27" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A28" s="7"/>
       <c r="B28" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A29" s="7"/>
       <c r="B29" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A30" s="7"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A31" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A32" s="7"/>
       <c r="B32" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A33" s="7"/>
       <c r="B33" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A34" s="7"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A35" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A36" s="7"/>
       <c r="B36" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A37" s="7"/>
       <c r="B37" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A38" s="7"/>
       <c r="B38" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A39" s="7"/>
       <c r="B39" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A40" s="7"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A41" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A42" s="7"/>
       <c r="B42" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A43" s="7"/>
       <c r="B43" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A44" s="7"/>
       <c r="B44" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A45" s="7"/>
       <c r="B45" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A46" s="7"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A47" s="7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A48" s="7"/>
       <c r="B48" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A49" s="7"/>
       <c r="B49" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A50" s="7"/>
       <c r="B50" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A51" s="7"/>
       <c r="B51" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A52" s="7"/>
       <c r="B52" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A53" s="7"/>
       <c r="B53" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A54" s="7"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A55" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A56" s="7"/>
       <c r="B56" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A57" s="7"/>
       <c r="B57" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A58" s="7"/>
       <c r="B58" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A59" s="7"/>
       <c r="B59" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A60" s="7"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A61" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A62" s="7"/>
       <c r="B62" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A63" s="7"/>
       <c r="B63" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A64" s="7"/>
       <c r="B64" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A65" s="7"/>
       <c r="B65" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A66" s="7"/>
       <c r="B66" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A67" s="7"/>
       <c r="B67" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
       <c r="F67" s="5"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A68" s="7"/>
       <c r="B68" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A69" s="7"/>
       <c r="B69" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A70" s="7"/>
       <c r="B70" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A71" s="7"/>
       <c r="B71" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A72" s="7"/>
       <c r="B72" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A73" s="7"/>
       <c r="B73" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A74" s="7"/>
       <c r="B74" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A75" s="7"/>
       <c r="B75" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A76" s="7"/>
       <c r="B76" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A77" s="7"/>
       <c r="B77" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
       <c r="E77" s="5"/>
       <c r="F77" s="5"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A78" s="7"/>
       <c r="B78" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A79" s="7"/>
       <c r="B79" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A80" s="7"/>
       <c r="B80" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>

</xml_diff>

<commit_message>
For now the change with the less impact
</commit_message>
<xml_diff>
--- a/tests/fixtures/excel/shipments-odcs.xlsx
+++ b/tests/fixtures/excel/shipments-odcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\datacontract-github-dev\datacontract-cli\tests\fixtures\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C652B2F-5E5B-4010-A683-FED37E0A5BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42AF7A54-A823-4EAD-A8DE-62119E23BB81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="266">
   <si>
     <t>Property</t>
   </si>
@@ -935,10 +935,10 @@
     <t>Table shall contain at least 1 row</t>
   </si>
   <si>
-    <t>mustBeGreaterThanOrEqualTo</t>
-  </si>
-  <si>
     <t>{field} must contain the field "destination"</t>
+  </si>
+  <si>
+    <t>mustBeGreaterOrEqualTo</t>
   </si>
 </sst>
 </file>
@@ -4412,8 +4412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0F4C5A-BE41-6140-9B9B-80B8DB7D1AD7}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.45"/>
@@ -4506,11 +4506,11 @@
       <c r="F5" s="37" t="s">
         <v>235</v>
       </c>
-      <c r="G5" s="37" t="s">
-        <v>264</v>
-      </c>
-      <c r="H5" s="37" t="s">
-        <v>236</v>
+      <c r="G5" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="H5" s="37">
+        <v>1</v>
       </c>
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
@@ -4529,7 +4529,7 @@
         <v>190</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="39"/>
@@ -4599,9 +4599,9 @@
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="15"/>
-      <c r="D9" s="17"/>
+      <c r="D9" s="35"/>
       <c r="E9" s="15"/>
-      <c r="F9" s="27"/>
+      <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
@@ -4825,6 +4825,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
implementation of mustBeGreaterOrEqualTo which is supported in the excel, aswell modification for whole numbers. Added unittest scenarios for fixed types
</commit_message>
<xml_diff>
--- a/tests/fixtures/excel/shipments-odcs.xlsx
+++ b/tests/fixtures/excel/shipments-odcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\datacontract-github-dev\datacontract-cli\tests\fixtures\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42AF7A54-A823-4EAD-A8DE-62119E23BB81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D316ADF1-8766-4715-B007-DB5AD54C7BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="277">
   <si>
     <t>Property</t>
   </si>
@@ -920,25 +920,58 @@
     <t>mustBe</t>
   </si>
   <si>
-    <t>confirming that the total number of records divided by 2 is 3.5</t>
-  </si>
-  <si>
-    <t>confirming that the total number of records  is 7</t>
-  </si>
-  <si>
     <t>1.0.2</t>
   </si>
   <si>
     <t>SELECT AVG(duration) FROM shipments</t>
   </si>
   <si>
-    <t>Table shall contain at least 1 row</t>
-  </si>
-  <si>
     <t>{field} must contain the field "destination"</t>
   </si>
   <si>
     <t>mustBeGreaterOrEqualTo</t>
+  </si>
+  <si>
+    <t>mustBeLessThan</t>
+  </si>
+  <si>
+    <t>mustBeLessOrEqualTo</t>
+  </si>
+  <si>
+    <t>mustBeBetween</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) FROM shipments where carries='active'</t>
+  </si>
+  <si>
+    <t>SELECT AVG(*) FROM shipments</t>
+  </si>
+  <si>
+    <t>6.8</t>
+  </si>
+  <si>
+    <t>testscenario for mustBe (integer)</t>
+  </si>
+  <si>
+    <t>testscenario for mustBe (float)</t>
+  </si>
+  <si>
+    <t>testscenario for mustBeLessThan (integer)</t>
+  </si>
+  <si>
+    <t>testscenario for mustBeLessThan (float)</t>
+  </si>
+  <si>
+    <t>testscenario for mustBeBetween</t>
+  </si>
+  <si>
+    <t>testscenario for mustBeGreaterOrEqualTo</t>
+  </si>
+  <si>
+    <t>[25,75]</t>
   </si>
 </sst>
 </file>
@@ -1177,7 +1210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1264,9 +1297,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2300,7 +2330,7 @@
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="34" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.5">
@@ -2317,10 +2347,10 @@
       <c r="B11" s="7"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="41"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="5" t="s">
         <v>168</v>
       </c>
@@ -2475,78 +2505,78 @@
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="41" t="s">
         <v>173</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="41" t="s">
         <v>176</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="42" t="s">
         <v>165</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="45"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="44"/>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A9" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="42" t="s">
         <v>174</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="45"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="44"/>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A10" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="45"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="44"/>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="41" t="s">
         <v>177</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.5">
       <c r="W12" s="19" t="s">
@@ -4412,8 +4442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0F4C5A-BE41-6140-9B9B-80B8DB7D1AD7}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.45"/>
@@ -4421,7 +4451,7 @@
     <col min="1" max="1" width="17.46484375" style="30" customWidth="1"/>
     <col min="2" max="2" width="22" style="30" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" style="30" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" style="30" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" style="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" style="30" customWidth="1"/>
     <col min="6" max="6" width="28.33203125" style="30" customWidth="1"/>
     <col min="7" max="7" width="19" style="30" bestFit="1" customWidth="1"/>
@@ -4451,7 +4481,7 @@
       <c r="B3" s="31"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="35" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="32" t="s">
@@ -4492,24 +4522,24 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="31.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="37" t="s">
+      <c r="B5" s="37"/>
+      <c r="C5" s="36" t="s">
         <v>234</v>
       </c>
-      <c r="D5" s="37" t="s">
-        <v>263</v>
-      </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37" t="s">
+      <c r="D5" s="17" t="s">
+        <v>275</v>
+      </c>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36" t="s">
         <v>235</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>265</v>
-      </c>
-      <c r="H5" s="37">
+        <v>262</v>
+      </c>
+      <c r="H5" s="36">
         <v>1</v>
       </c>
       <c r="I5" s="15"/>
@@ -4519,22 +4549,22 @@
       <c r="M5" s="15"/>
     </row>
     <row r="6" spans="1:13" ht="31.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="37" t="s">
         <v>211</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="D6" s="37" t="s">
-        <v>264</v>
-      </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
+      <c r="D6" s="36" t="s">
+        <v>261</v>
+      </c>
+      <c r="E6" s="36"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
@@ -4549,8 +4579,8 @@
       <c r="C7" s="15" t="s">
         <v>234</v>
       </c>
-      <c r="D7" s="35" t="s">
-        <v>260</v>
+      <c r="D7" s="17" t="s">
+        <v>270</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15" t="s">
@@ -4562,11 +4592,11 @@
       <c r="H7" s="15">
         <v>7</v>
       </c>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-      <c r="M7" s="37"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="36"/>
     </row>
     <row r="8" spans="1:13" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A8" s="17" t="s">
@@ -4576,64 +4606,100 @@
       <c r="C8" s="15" t="s">
         <v>234</v>
       </c>
-      <c r="D8" s="35" t="s">
-        <v>259</v>
+      <c r="D8" s="17" t="s">
+        <v>271</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>258</v>
       </c>
-      <c r="H8" s="15">
-        <v>3.5</v>
-      </c>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="37"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
+      <c r="H8" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+    </row>
+    <row r="9" spans="1:13" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="A9" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" s="37"/>
+      <c r="C9" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36" t="s">
+        <v>267</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="H9" s="36">
+        <v>1</v>
+      </c>
       <c r="I9" s="15"/>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
       <c r="M9" s="15"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
+    <row r="10" spans="1:13" ht="31.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="B10" s="37"/>
+      <c r="C10" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36" t="s">
+        <v>260</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="H10" s="36" t="s">
+        <v>269</v>
+      </c>
       <c r="I10" s="15"/>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
       <c r="L10" s="15"/>
       <c r="M10" s="15"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
+    <row r="11" spans="1:13" ht="31.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="B11" s="37"/>
+      <c r="C11" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36" t="s">
+        <v>268</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="H11" s="36" t="s">
+        <v>276</v>
+      </c>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>

</xml_diff>

<commit_message>
Export and Import Excel to (ODCS v3) YAML Bug Fixes (#956)
* Fix for generating corrupted yaml when importing from excel using the mustBe and mustBeNot expectations.

* merged wrong idention

* recovered incorrect commit

* For now the change with the less impact

* implementation of mustBeGreaterOrEqualTo which is supported in the excel, aswell modification for whole numbers. Added unittest scenarios for fixed types

---------

Co-authored-by: Christian van Rodijnen <christian.vanrodijnen@surf.nl>
</commit_message>
<xml_diff>
--- a/tests/fixtures/excel/shipments-odcs.xlsx
+++ b/tests/fixtures/excel/shipments-odcs.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jochen/Projects/open-data-contract-standard-excel-template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\datacontract-github-dev\datacontract-cli\tests\fixtures\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58ECC940-E1E1-584B-B311-B4AA053E9340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D316ADF1-8766-4715-B007-DB5AD54C7BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="1"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="8" r:id="rId1"/>
     <sheet name="Fundamentals" sheetId="10" r:id="rId2"/>
-    <sheet name="Schema shipments" r:id="rId16" sheetId="22"/>
+    <sheet name="Schema shipments" sheetId="22" r:id="rId3"/>
     <sheet name="Quality" sheetId="21" r:id="rId4"/>
     <sheet name="Support" sheetId="12" r:id="rId5"/>
     <sheet name="Team" sheetId="13" r:id="rId6"/>
@@ -44,6 +44,14 @@
     <definedName name="price.priceUnit">Pricing!$B$6</definedName>
     <definedName name="quality">Quality!$A$4:$AZ$300</definedName>
     <definedName name="roles" localSheetId="6">Roles!$A$4:$E$1000</definedName>
+    <definedName name="schema.businessName" localSheetId="2">'Schema shipments'!$B$8</definedName>
+    <definedName name="schema.dataGranularityDescription" localSheetId="2">'Schema shipments'!$B$10</definedName>
+    <definedName name="schema.description" localSheetId="2">'Schema shipments'!$B$7</definedName>
+    <definedName name="schema.name" localSheetId="2">'Schema shipments'!$B$5</definedName>
+    <definedName name="schema.physicalName" localSheetId="2">'Schema shipments'!$B$9</definedName>
+    <definedName name="schema.physicalType" localSheetId="2">'Schema shipments'!$B$6</definedName>
+    <definedName name="schema.properties" localSheetId="2">'Schema shipments'!$A$13:$L$981</definedName>
+    <definedName name="schema.tags" localSheetId="2">'Schema shipments'!$B$11</definedName>
     <definedName name="servers.azure.delimiter">Servers!$C$14</definedName>
     <definedName name="servers.azure.format">Servers!$C$13</definedName>
     <definedName name="servers.azure.location">Servers!$C$12</definedName>
@@ -107,16 +115,8 @@
     <definedName name="team">Team!$A$4:$G$1000</definedName>
     <definedName name="tenant">Fundamentals!$C$16</definedName>
     <definedName name="version">Fundamentals!$C$9</definedName>
-    <definedName name="schema.businessName" localSheetId="2">'Schema shipments'!$B$8</definedName>
-    <definedName name="schema.dataGranularityDescription" localSheetId="2">'Schema shipments'!$B$10</definedName>
-    <definedName name="schema.description" localSheetId="2">'Schema shipments'!$B$7</definedName>
-    <definedName name="schema.name" localSheetId="2">'Schema shipments'!$B$5</definedName>
-    <definedName name="schema.physicalName" localSheetId="2">'Schema shipments'!$B$9</definedName>
-    <definedName name="schema.physicalType" localSheetId="2">'Schema shipments'!$B$6</definedName>
-    <definedName name="schema.properties" localSheetId="2">'Schema shipments'!$A$13:$L$981</definedName>
-    <definedName name="schema.tags" localSheetId="2">'Schema shipments'!$B$11</definedName>
   </definedNames>
-  <calcPr calcId="191029" fullCalcOnLoad="true"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="277">
   <si>
     <t>Property</t>
   </si>
@@ -154,9 +154,6 @@
     <t>apiVersion</t>
   </si>
   <si>
-    <t>v3.0.2</t>
-  </si>
-  <si>
     <t>Logical Type</t>
   </si>
   <si>
@@ -290,9 +287,6 @@
   </si>
   <si>
     <t>Copy this sheet for every model in your data contract.</t>
-  </si>
-  <si>
-    <t>&lt;table_name&gt;</t>
   </si>
   <si>
     <t>Physical Name</t>
@@ -647,9 +641,6 @@
     <t>Shipments</t>
   </si>
   <si>
-    <t>1.0.1</t>
-  </si>
-  <si>
     <t>draft</t>
   </si>
   <si>
@@ -857,90 +848,137 @@
     <t>sql</t>
   </si>
   <si>
-    <t>Table shall contain at least 1 row</t>
-  </si>
-  <si>
     <t>SELECT COUNT(*) FROM shipments</t>
   </si>
   <si>
-    <t>mustBeGreaterThanOrEqualTo</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
+    <t>additionalField</t>
+  </si>
+  <si>
+    <t>We added an addition field - b</t>
+  </si>
+  <si>
+    <t>slackname</t>
+  </si>
+  <si>
+    <t>http://find.me.here</t>
+  </si>
+  <si>
+    <t>slack</t>
+  </si>
+  <si>
+    <t>interactive</t>
+  </si>
+  <si>
+    <t>vimportant</t>
+  </si>
+  <si>
+    <t>administrator</t>
+  </si>
+  <si>
+    <t>2020-01-01</t>
+  </si>
+  <si>
+    <t>nimportant</t>
+  </si>
+  <si>
+    <t>reader</t>
+  </si>
+  <si>
+    <t>2024-10-10</t>
+  </si>
+  <si>
+    <t>availability</t>
+  </si>
+  <si>
+    <t>95%</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>operational</t>
+  </si>
+  <si>
+    <t>production</t>
+  </si>
+  <si>
+    <t>bigquery</t>
+  </si>
+  <si>
+    <t>acme_shipments_prod</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>Per 1000 requests</t>
+  </si>
+  <si>
+    <t>mustBe</t>
+  </si>
+  <si>
+    <t>1.0.2</t>
+  </si>
+  <si>
+    <t>SELECT AVG(duration) FROM shipments</t>
+  </si>
+  <si>
     <t>{field} must contain the field "destination"</t>
   </si>
   <si>
-    <t>additionalField</t>
-  </si>
-  <si>
-    <t>We added an addition field - b</t>
-  </si>
-  <si>
-    <t>slackname</t>
-  </si>
-  <si>
-    <t>http://find.me.here</t>
-  </si>
-  <si>
-    <t>slack</t>
-  </si>
-  <si>
-    <t>interactive</t>
-  </si>
-  <si>
-    <t>vimportant</t>
-  </si>
-  <si>
-    <t>administrator</t>
-  </si>
-  <si>
-    <t>2020-01-01</t>
-  </si>
-  <si>
-    <t>nimportant</t>
-  </si>
-  <si>
-    <t>reader</t>
-  </si>
-  <si>
-    <t>2024-10-10</t>
-  </si>
-  <si>
-    <t>availability</t>
-  </si>
-  <si>
-    <t>95%</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>operational</t>
-  </si>
-  <si>
-    <t>production</t>
-  </si>
-  <si>
-    <t>bigquery</t>
-  </si>
-  <si>
-    <t>acme_shipments_prod</t>
-  </si>
-  <si>
-    <t>EUR</t>
-  </si>
-  <si>
-    <t>Per 1000 requests</t>
+    <t>mustBeGreaterOrEqualTo</t>
+  </si>
+  <si>
+    <t>mustBeLessThan</t>
+  </si>
+  <si>
+    <t>mustBeLessOrEqualTo</t>
+  </si>
+  <si>
+    <t>mustBeBetween</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) FROM shipments where carries='active'</t>
+  </si>
+  <si>
+    <t>SELECT AVG(*) FROM shipments</t>
+  </si>
+  <si>
+    <t>6.8</t>
+  </si>
+  <si>
+    <t>testscenario for mustBe (integer)</t>
+  </si>
+  <si>
+    <t>testscenario for mustBe (float)</t>
+  </si>
+  <si>
+    <t>testscenario for mustBeLessThan (integer)</t>
+  </si>
+  <si>
+    <t>testscenario for mustBeLessThan (float)</t>
+  </si>
+  <si>
+    <t>testscenario for mustBeBetween</t>
+  </si>
+  <si>
+    <t>testscenario for mustBeGreaterOrEqualTo</t>
+  </si>
+  <si>
+    <t>[25,75]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -990,6 +1028,25 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Mono"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1153,7 +1210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1223,6 +1280,36 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1240,21 +1327,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1639,42 +1711,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView topLeftCell="A9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="14.0"/>
-    <col min="2" max="16384" style="3" width="8.83203125"/>
+    <col min="1" max="1" width="14" style="3" customWidth="1"/>
+    <col min="2" max="16384" width="8.796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A2" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A7" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -1685,9 +1757,9 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A8" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -1698,9 +1770,9 @@
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A9" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -1711,9 +1783,9 @@
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
     </row>
-    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A10" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
@@ -1724,9 +1796,9 @@
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A11" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
@@ -1737,7 +1809,7 @@
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
@@ -1748,7 +1820,7 @@
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
     </row>
-    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -1759,9 +1831,9 @@
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A14" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -1772,9 +1844,9 @@
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A15" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -1785,9 +1857,9 @@
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A16" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
@@ -1798,9 +1870,9 @@
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
     </row>
-    <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A17" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
@@ -1811,12 +1883,12 @@
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
     </row>
-    <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A18" s="23" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
@@ -1826,10 +1898,10 @@
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
     </row>
-    <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A19" s="23"/>
       <c r="B19" s="24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
@@ -1839,7 +1911,7 @@
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
     </row>
-    <row r="20" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A20" s="13"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
@@ -1850,12 +1922,12 @@
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
     </row>
-    <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A21" s="25" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
@@ -1865,10 +1937,10 @@
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
     </row>
-    <row r="22" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A22" s="25"/>
       <c r="B22" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
@@ -1878,10 +1950,10 @@
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
     </row>
-    <row r="23" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A23" s="13"/>
       <c r="B23" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
@@ -1891,10 +1963,10 @@
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
     </row>
-    <row r="24" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A24" s="13"/>
       <c r="B24" s="13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
@@ -1904,7 +1976,7 @@
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
     </row>
-    <row r="25" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
@@ -1915,12 +1987,12 @@
       <c r="H25" s="13"/>
       <c r="I25" s="13"/>
     </row>
-    <row r="26" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A26" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="13" t="s">
         <v>40</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>41</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
@@ -1930,12 +2002,12 @@
       <c r="H26" s="13"/>
       <c r="I26" s="13"/>
     </row>
-    <row r="27" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A27" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
@@ -1945,12 +2017,12 @@
       <c r="H27" s="13"/>
       <c r="I27" s="13"/>
     </row>
-    <row r="28" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A28" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="13" t="s">
         <v>42</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>43</v>
       </c>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
@@ -1960,7 +2032,7 @@
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
@@ -1971,7 +2043,7 @@
       <c r="H29" s="13"/>
       <c r="I29" s="13"/>
     </row>
-    <row r="30" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
@@ -1982,7 +2054,7 @@
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
     </row>
-    <row r="31" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -1995,10 +2067,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B24" r:id="rId2"/>
+    <hyperlink ref="B24" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2008,46 +2080,46 @@
   <sheetViews>
     <sheetView zoomScale="165" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="22" width="26.1640625"/>
-    <col min="2" max="2" customWidth="true" style="22" width="22.33203125"/>
-    <col min="3" max="16384" style="22" width="10.83203125"/>
+    <col min="1" max="1" width="26.1328125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="22" customWidth="1"/>
+    <col min="3" max="16384" width="10.796875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="2" customFormat="1" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A2" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.5"/>
+    <row r="4" spans="1:2" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A4" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A5" s="7" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:2" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="B5" s="5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A6" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>94</v>
-      </c>
       <c r="B6" s="5" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -2068,24 +2140,24 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="33.1640625"/>
-    <col min="2" max="2" customWidth="true" style="2" width="90.0"/>
-    <col min="3" max="16384" style="2" width="8.83203125"/>
+    <col min="1" max="1" width="33.1328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="90" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A2" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
@@ -2093,80 +2165,80 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A5" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="5" t="str">
         <f>IF(owner&lt;&gt;"",owner,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>fulfillment</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A6" s="5" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
     </row>
@@ -2183,184 +2255,184 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="2.83203125"/>
-    <col min="2" max="2" customWidth="true" style="2" width="19.6640625"/>
-    <col min="3" max="3" customWidth="true" style="2" width="45.0"/>
-    <col min="4" max="4" customWidth="true" style="2" width="1.83203125"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="28.1640625"/>
-    <col min="6" max="6" customWidth="true" style="2" width="14.33203125"/>
-    <col min="7" max="8" customWidth="true" style="2" width="10.0"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="14.1640625"/>
-    <col min="10" max="11" customWidth="true" style="2" width="14.33203125"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="23.5"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="24.1640625"/>
-    <col min="14" max="16384" style="2" width="8.83203125"/>
+    <col min="1" max="1" width="2.796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="45" style="2" customWidth="1"/>
+    <col min="4" max="4" width="1.796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="2" customWidth="1"/>
+    <col min="7" max="8" width="10" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="14.33203125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="23.46484375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A2" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A4" s="7" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A7" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A8" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="34" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A10" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="30"/>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A12" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="40"/>
       <c r="C12" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A14" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="5"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A15" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="5"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A16" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A18" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="7"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A19" s="7"/>
       <c r="B19" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A20" s="7"/>
       <c r="B20" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A21" s="7"/>
       <c r="B21" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A23" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -2382,131 +2454,133 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AL49"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="100" workbookViewId="0" tabSelected="false"/>
+    <sheetView zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:E5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="34.83203125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="24.0"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.5"/>
-    <col min="4" max="4" customWidth="true" style="2" width="17.5"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="8" width="28.1640625"/>
-    <col min="6" max="6" customWidth="true" style="2" width="35.6640625"/>
-    <col min="7" max="8" customWidth="true" style="2" width="10.0"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="14.1640625"/>
-    <col min="10" max="10" customWidth="true" style="2" width="14.33203125"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="28.1640625"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="28.6640625"/>
-    <col min="13" max="13" customWidth="true" style="2" width="28.6640625"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="11.6640625"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="19.0"/>
-    <col min="16" max="20" customWidth="true" style="2" width="19.0"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="2" width="21.6640625"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="2" width="27.33203125"/>
-    <col min="23" max="37" customWidth="true" style="2" width="15.5"/>
-    <col min="38" max="38" customWidth="true" style="2" width="26.1640625"/>
-    <col min="39" max="16384" style="2" width="8.83203125"/>
+    <col min="1" max="1" width="34.796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.46484375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.46484375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.1328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" style="2" customWidth="1"/>
+    <col min="7" max="8" width="10" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="28.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.6640625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="20" width="19" style="2" customWidth="1"/>
+    <col min="21" max="21" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="37" width="15.46484375" style="2" customWidth="1"/>
+    <col min="38" max="38" width="26.1328125" style="2" customWidth="1"/>
+    <col min="39" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.5">
+      <c r="A2" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.5">
+      <c r="A3" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.5">
+      <c r="A5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>173</v>
+      </c>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.5">
+      <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>176</v>
-      </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-    </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-    </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="B6" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="31" t="s">
-        <v>179</v>
-      </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-    </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="B7" s="41" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="34"/>
-    </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="44"/>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A9" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="44"/>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.5">
+      <c r="A10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="44"/>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.5">
+      <c r="A11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="41" t="s">
         <v>177</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="34"/>
-    </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>178</v>
-      </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="34"/>
-    </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>180</v>
-      </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-    </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.5">
       <c r="W12" s="19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="X12" s="20"/>
       <c r="Y12" s="20"/>
@@ -2523,21 +2597,21 @@
       <c r="AJ12" s="20"/>
       <c r="AK12" s="21"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A13" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>10</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>11</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>3</v>
@@ -2546,117 +2620,117 @@
         <v>2</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="K13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="K13" s="10" t="s">
+      <c r="L13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="L13" s="10" t="s">
-        <v>15</v>
-      </c>
       <c r="M13" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N13" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="O13" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="P13" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q13" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="O13" s="10" t="s">
+      <c r="R13" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="P13" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q13" s="10" t="s">
+      <c r="S13" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="R13" s="10" t="s">
+      <c r="T13" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="S13" s="10" t="s">
+      <c r="U13" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="T13" s="10" t="s">
+      <c r="V13" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="U13" s="10" t="s">
+      <c r="W13" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="V13" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="W13" s="10" t="s">
+      <c r="X13" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="X13" s="10" t="s">
+      <c r="Y13" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z13" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="Y13" s="10" t="s">
+      <c r="AA13" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB13" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC13" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="AD13" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE13" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="Z13" s="10" t="s">
+      <c r="AF13" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="AA13" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB13" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="AC13" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="AD13" s="10" t="s">
+      <c r="AG13" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH13" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="AI13" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="AE13" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="AF13" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="AG13" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="AH13" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="AI13" s="10" t="s">
+      <c r="AJ13" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="AK13" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="AJ13" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="AK13" s="10" t="s">
-        <v>89</v>
-      </c>
       <c r="AL13" s="10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A14" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="E14" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="F14" s="15" t="s">
         <v>183</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>186</v>
       </c>
       <c r="G14" s="15" t="b">
         <v>0</v>
@@ -2665,19 +2739,19 @@
         <v>0</v>
       </c>
       <c r="I14" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="L14" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="J14" s="15" t="s">
+      <c r="M14" s="15" t="s">
         <v>188</v>
-      </c>
-      <c r="K14" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="L14" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="M14" s="15" t="s">
-        <v>191</v>
       </c>
       <c r="N14" s="15" t="b">
         <v>1</v>
@@ -2711,14 +2785,14 @@
       <c r="AK14" s="15"/>
       <c r="AL14" s="28"/>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:38" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A15" s="17" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E15" s="16"/>
       <c r="F15" s="15"/>
@@ -2727,13 +2801,13 @@
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
       <c r="K15" s="15" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="L15" s="15" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="M15" s="15" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="N15" s="15" t="b">
         <v>0</v>
@@ -2765,24 +2839,24 @@
       <c r="AK15" s="15"/>
       <c r="AL15" s="28"/>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:38" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A16" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="D16" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="E16" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="F16" s="15" t="s">
         <v>198</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>201</v>
       </c>
       <c r="G16" s="15" t="b">
         <v>0</v>
@@ -2791,7 +2865,7 @@
         <v>0</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
@@ -2829,24 +2903,24 @@
       <c r="AK16" s="15"/>
       <c r="AL16" s="28"/>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:38" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A17" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="F17" s="15" t="s">
         <v>202</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>205</v>
       </c>
       <c r="G17" s="15" t="b">
         <v>0</v>
@@ -2855,7 +2929,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
@@ -2893,24 +2967,24 @@
       <c r="AK17" s="15"/>
       <c r="AL17" s="28"/>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:38" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A18" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="F18" s="15" t="s">
         <v>206</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>209</v>
       </c>
       <c r="G18" s="15" t="b">
         <v>0</v>
@@ -2919,7 +2993,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
@@ -2957,24 +3031,24 @@
       <c r="AK18" s="15"/>
       <c r="AL18" s="28"/>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A19" s="17" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G19" s="15" t="b">
         <v>0</v>
@@ -2983,7 +3057,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
@@ -3021,24 +3095,24 @@
       <c r="AK19" s="15"/>
       <c r="AL19" s="28"/>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:38" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A20" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="D20" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="E20" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="F20" s="15" t="s">
         <v>216</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>218</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>219</v>
       </c>
       <c r="G20" s="15" t="b">
         <v>0</v>
@@ -3047,7 +3121,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
@@ -3061,7 +3135,7 @@
         <v>0</v>
       </c>
       <c r="Q20" s="15" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="R20" s="15"/>
       <c r="S20" s="15"/>
@@ -3087,29 +3161,29 @@
       <c r="AK20" s="15"/>
       <c r="AL20" s="28"/>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A21" s="18" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E21" s="16"/>
       <c r="F21" s="15" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G21" s="15" t="b">
         <v>1</v>
       </c>
       <c r="H21" s="15"/>
       <c r="I21" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
@@ -3141,24 +3215,24 @@
       <c r="AK21" s="15"/>
       <c r="AL21" s="28"/>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A22" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="F22" s="15" t="s">
         <v>225</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>226</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>228</v>
       </c>
       <c r="G22" s="15" t="b">
         <v>1</v>
@@ -3167,7 +3241,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J22" s="15"/>
       <c r="K22" s="15"/>
@@ -3203,24 +3277,24 @@
       <c r="AK22" s="15"/>
       <c r="AL22" s="28"/>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A23" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="F23" s="15" t="s">
         <v>229</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>230</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>231</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>232</v>
       </c>
       <c r="G23" s="15" t="b">
         <v>1</v>
@@ -3229,7 +3303,7 @@
         <v>0</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J23" s="15"/>
       <c r="K23" s="15"/>
@@ -3265,31 +3339,31 @@
       <c r="AK23" s="15"/>
       <c r="AL23" s="28"/>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A24" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="F24" s="15" t="s">
         <v>233</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>234</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>235</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>236</v>
       </c>
       <c r="G24" s="15" t="b">
         <v>1</v>
       </c>
       <c r="H24" s="15"/>
       <c r="I24" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J24" s="15"/>
       <c r="K24" s="15"/>
@@ -3325,7 +3399,7 @@
       <c r="AK24" s="15"/>
       <c r="AL24" s="28"/>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A25" s="17"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
@@ -3365,7 +3439,7 @@
       <c r="AK25" s="15"/>
       <c r="AL25" s="28"/>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A26" s="17"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -3405,7 +3479,7 @@
       <c r="AK26" s="15"/>
       <c r="AL26" s="28"/>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A27" s="17"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
@@ -3445,7 +3519,7 @@
       <c r="AK27" s="15"/>
       <c r="AL27" s="28"/>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A28" s="17"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -3485,7 +3559,7 @@
       <c r="AK28" s="15"/>
       <c r="AL28" s="28"/>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A29" s="17"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -3525,7 +3599,7 @@
       <c r="AK29" s="15"/>
       <c r="AL29" s="28"/>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A30" s="17"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -3565,7 +3639,7 @@
       <c r="AK30" s="15"/>
       <c r="AL30" s="28"/>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A31" s="17"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -3605,7 +3679,7 @@
       <c r="AK31" s="15"/>
       <c r="AL31" s="28"/>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A32" s="17"/>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -3645,7 +3719,7 @@
       <c r="AK32" s="15"/>
       <c r="AL32" s="28"/>
     </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A33" s="17"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -3685,7 +3759,7 @@
       <c r="AK33" s="15"/>
       <c r="AL33" s="28"/>
     </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A34" s="17"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -3725,7 +3799,7 @@
       <c r="AK34" s="15"/>
       <c r="AL34" s="28"/>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A35" s="17"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -3765,7 +3839,7 @@
       <c r="AK35" s="15"/>
       <c r="AL35" s="28"/>
     </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A36" s="17"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
@@ -3805,7 +3879,7 @@
       <c r="AK36" s="15"/>
       <c r="AL36" s="28"/>
     </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A37" s="17"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -3845,7 +3919,7 @@
       <c r="AK37" s="15"/>
       <c r="AL37" s="28"/>
     </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A38" s="17"/>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
@@ -3885,7 +3959,7 @@
       <c r="AK38" s="15"/>
       <c r="AL38" s="28"/>
     </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A39" s="17"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -3925,7 +3999,7 @@
       <c r="AK39" s="15"/>
       <c r="AL39" s="28"/>
     </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A40" s="17"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
@@ -3965,7 +4039,7 @@
       <c r="AK40" s="15"/>
       <c r="AL40" s="28"/>
     </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A41" s="17"/>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
@@ -4005,7 +4079,7 @@
       <c r="AK41" s="15"/>
       <c r="AL41" s="28"/>
     </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A42" s="17"/>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
@@ -4045,7 +4119,7 @@
       <c r="AK42" s="15"/>
       <c r="AL42" s="28"/>
     </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A43" s="17"/>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
@@ -4085,7 +4159,7 @@
       <c r="AK43" s="15"/>
       <c r="AL43" s="28"/>
     </row>
-    <row r="44" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A44" s="17"/>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
@@ -4125,7 +4199,7 @@
       <c r="AK44" s="15"/>
       <c r="AL44" s="28"/>
     </row>
-    <row r="45" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A45" s="17"/>
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
@@ -4165,7 +4239,7 @@
       <c r="AK45" s="15"/>
       <c r="AL45" s="28"/>
     </row>
-    <row r="46" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A46" s="17"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
@@ -4205,7 +4279,7 @@
       <c r="AK46" s="15"/>
       <c r="AL46" s="28"/>
     </row>
-    <row r="47" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A47" s="17"/>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
@@ -4245,7 +4319,7 @@
       <c r="AK47" s="15"/>
       <c r="AL47" s="28"/>
     </row>
-    <row r="48" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A48" s="17"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -4285,7 +4359,7 @@
       <c r="AK48" s="15"/>
       <c r="AL48" s="28"/>
     </row>
-    <row r="49" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A49" s="17"/>
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
@@ -4368,105 +4442,105 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0F4C5A-BE41-6140-9B9B-80B8DB7D1AD7}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="36" width="17.5"/>
-    <col min="2" max="2" customWidth="true" style="36" width="22.0"/>
-    <col min="3" max="3" customWidth="true" style="36" width="14.33203125"/>
-    <col min="4" max="4" customWidth="true" style="36" width="32.6640625"/>
-    <col min="5" max="5" customWidth="true" style="36" width="18.33203125"/>
-    <col min="6" max="6" customWidth="true" style="36" width="28.33203125"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="36" width="19.0"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="36" width="16.0"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="36" width="22.83203125"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="36" width="23.5"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="36" width="15.5"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="36" width="17.83203125"/>
-    <col min="13" max="13" customWidth="true" style="36" width="17.83203125"/>
-    <col min="14" max="16384" style="36" width="8.83203125"/>
+    <col min="1" max="1" width="17.46484375" style="30" customWidth="1"/>
+    <col min="2" max="2" width="22" style="30" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="30" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" style="30" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" style="30" customWidth="1"/>
+    <col min="7" max="7" width="19" style="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" style="30" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.796875" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.46484375" style="30" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.46484375" style="30" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.796875" style="30" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.796875" style="30" customWidth="1"/>
+    <col min="14" max="16384" width="8.796875" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:13" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="A1" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" s="29"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A2" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="31"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A4" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="G4" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="35"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
+      <c r="H4" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="B2" s="37"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="39" t="s">
+      <c r="I4" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="J4" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="K4" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="L4" s="33" t="s">
         <v>159</v>
       </c>
-      <c r="F4" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="G4" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="H4" s="39" t="s">
-        <v>155</v>
-      </c>
-      <c r="I4" s="39" t="s">
-        <v>158</v>
-      </c>
-      <c r="J4" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="K4" s="39" t="s">
+      <c r="M4" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="L4" s="39" t="s">
-        <v>161</v>
-      </c>
-      <c r="M4" s="39" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="15" t="s">
-        <v>237</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15" t="s">
-        <v>239</v>
+    </row>
+    <row r="5" spans="1:13" ht="31.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" s="37"/>
+      <c r="C5" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>275</v>
+      </c>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36" t="s">
+        <v>235</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>240</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>241</v>
+        <v>262</v>
+      </c>
+      <c r="H5" s="36">
+        <v>1</v>
       </c>
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
@@ -4474,109 +4548,169 @@
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
+    <row r="6" spans="1:13" ht="31.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>211</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>190</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>261</v>
+      </c>
+      <c r="E6" s="36"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
+    <row r="7" spans="1:13" ht="31.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="17" t="s">
+        <v>173</v>
+      </c>
       <c r="B7" s="17"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
+      <c r="C7" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>270</v>
+      </c>
       <c r="E7" s="15"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="17"/>
+      <c r="F7" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="H7" s="15">
+        <v>7</v>
+      </c>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="36"/>
+    </row>
+    <row r="8" spans="1:13" ht="31.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="17" t="s">
+        <v>173</v>
+      </c>
       <c r="B8" s="17"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
+      <c r="C8" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>271</v>
+      </c>
       <c r="E8" s="15"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
+      <c r="F8" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+    </row>
+    <row r="9" spans="1:13" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="A9" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" s="37"/>
+      <c r="C9" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36" t="s">
+        <v>267</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="H9" s="36">
+        <v>1</v>
+      </c>
       <c r="I9" s="15"/>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
       <c r="M9" s="15"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
+    <row r="10" spans="1:13" ht="31.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="B10" s="37"/>
+      <c r="C10" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36" t="s">
+        <v>260</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="H10" s="36" t="s">
+        <v>269</v>
+      </c>
       <c r="I10" s="15"/>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
       <c r="L10" s="15"/>
       <c r="M10" s="15"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
+    <row r="11" spans="1:13" ht="31.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="B11" s="37"/>
+      <c r="C11" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36" t="s">
+        <v>268</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="H11" s="36" t="s">
+        <v>276</v>
+      </c>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
       <c r="M11" s="15"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
       <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
+      <c r="D12" s="17"/>
       <c r="E12" s="15"/>
       <c r="F12" s="27"/>
       <c r="G12" s="15"/>
@@ -4587,11 +4721,11 @@
       <c r="L12" s="15"/>
       <c r="M12" s="15"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
       <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
+      <c r="D13" s="17"/>
       <c r="E13" s="15"/>
       <c r="F13" s="27"/>
       <c r="G13" s="15"/>
@@ -4602,11 +4736,11 @@
       <c r="L13" s="15"/>
       <c r="M13" s="15"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="17"/>
       <c r="B14" s="17"/>
       <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
+      <c r="D14" s="17"/>
       <c r="E14" s="15"/>
       <c r="F14" s="27"/>
       <c r="G14" s="15"/>
@@ -4617,11 +4751,11 @@
       <c r="L14" s="15"/>
       <c r="M14" s="15"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="17"/>
       <c r="B15" s="17"/>
       <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
+      <c r="D15" s="17"/>
       <c r="E15" s="15"/>
       <c r="F15" s="27"/>
       <c r="G15" s="15"/>
@@ -4632,11 +4766,11 @@
       <c r="L15" s="15"/>
       <c r="M15" s="15"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
       <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
+      <c r="D16" s="17"/>
       <c r="E16" s="15"/>
       <c r="F16" s="27"/>
       <c r="G16" s="15"/>
@@ -4647,11 +4781,11 @@
       <c r="L16" s="15"/>
       <c r="M16" s="15"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
+      <c r="D17" s="17"/>
       <c r="E17" s="15"/>
       <c r="F17" s="27"/>
       <c r="G17" s="15"/>
@@ -4662,11 +4796,11 @@
       <c r="L17" s="15"/>
       <c r="M17" s="15"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
+      <c r="D18" s="17"/>
       <c r="E18" s="15"/>
       <c r="F18" s="27"/>
       <c r="G18" s="15"/>
@@ -4677,11 +4811,11 @@
       <c r="L18" s="15"/>
       <c r="M18" s="15"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="17"/>
       <c r="B19" s="17"/>
       <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
+      <c r="D19" s="17"/>
       <c r="E19" s="15"/>
       <c r="F19" s="27"/>
       <c r="G19" s="15"/>
@@ -4692,11 +4826,11 @@
       <c r="L19" s="15"/>
       <c r="M19" s="15"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="17"/>
       <c r="B20" s="17"/>
       <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
+      <c r="D20" s="17"/>
       <c r="E20" s="15"/>
       <c r="F20" s="27"/>
       <c r="G20" s="15"/>
@@ -4707,11 +4841,11 @@
       <c r="L20" s="15"/>
       <c r="M20" s="15"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="17"/>
       <c r="B21" s="17"/>
       <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
+      <c r="D21" s="17"/>
       <c r="E21" s="15"/>
       <c r="F21" s="27"/>
       <c r="G21" s="15"/>
@@ -4740,6 +4874,10 @@
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Severity" prompt="The severity of the data quality rule, such as error or warning." sqref="K5:K21" xr:uid="{0F4D661D-23D9-2540-B241-435A8E49610F}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Implementation" prompt="The data quality check in the engine's specific format." sqref="J5:J21" xr:uid="{00416CE8-FD1E-374C-B0CF-0FDCB1952802}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Engine" prompt="Required for custom DQ rule: name of the third-party engine being used. Any value is authorized here but common values are soda, greatExpectations, montecarlo, etc." sqref="I5:I21" xr:uid="{0459F568-8532-4048-9CA7-5708CD6DF179}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Schema" prompt="The schema name must match the name of the schema (table, ...) in the previous sheets." sqref="A4" xr:uid="{67CAE90D-676C-A44B-B965-361A399ACA9A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Property" prompt="Optional: Leave empty, if this is a schema-level quality check._x000a_The property must match the property name in the schema._x000a_" sqref="B4" xr:uid="{F3E67713-E117-6E46-AEFE-6861F5933838}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Rule" prompt="The predefined data quality rule from the library._x000a_Only appliable if &quot;Quality Type&quot; is set to &quot;library&quot; or empty (which is library by default, if a rule is defined)" sqref="E4" xr:uid="{4E8AA24F-1E70-FF4C-81CC-D9A25B05246C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality" prompt="The expected or guaranteed data quality from a business perspective._x000a__x000a_Maps to quality.description" sqref="D5:D21" xr:uid="{C84C6FF8-FC8D-B848-AC69-3DB82C6CB871}"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Threshold Value" prompt="The acutal value for the treshold operator._x000a_For mustBeBetween adn mustNotBeBetween, use [lowerBoundry, upperBoundy] syntax, e.g. [0, 100]." sqref="H5:H21" xr:uid="{E792E24E-6B57-A948-A026-4637119AD944}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Quality Operator" prompt="The comparation operator specifies the condition to validate the rule._x000a_Use it together with the threshold value, e.g. mustBe 0, or mustBeBetween [0,100]_x000a_This is applicable for quality type sql and some library rules." sqref="G5:G21" xr:uid="{15B1EE74-8A6D-3F49-A7EC-55C27203D116}">
       <formula1>"mustBe, mustNotBe, mustBeGreaterThan, mustBeGreaterOrEqualTo, mustBeLessThan, mustBeLessOrEqualTo, mustBeBetween, mustNotBeBetween"</formula1>
@@ -4751,12 +4889,9 @@
     <dataValidation type="list" allowBlank="1" sqref="C5:C21" xr:uid="{664F88A2-7556-9B4E-A851-8889D6576B99}">
       <formula1>"text,library,sql,custom"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality" prompt="The expected or guaranteed data quality from a business perspective._x000a__x000a_Maps to quality.description" sqref="D5:D21" xr:uid="{C84C6FF8-FC8D-B848-AC69-3DB82C6CB871}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Schema" prompt="The schema name must match the name of the schema (table, ...) in the previous sheets." sqref="A4" xr:uid="{67CAE90D-676C-A44B-B965-361A399ACA9A}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Property" prompt="Optional: Leave empty, if this is a schema-level quality check._x000a_The property must match the property name in the schema._x000a_" sqref="B4" xr:uid="{F3E67713-E117-6E46-AEFE-6861F5933838}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Rule" prompt="The predefined data quality rule from the library._x000a_Only appliable if &quot;Quality Type&quot; is set to &quot;library&quot; or empty (which is library by default, if a rule is defined)" sqref="E4" xr:uid="{4E8AA24F-1E70-FF4C-81CC-D9A25B05246C}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4768,61 +4903,61 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="33.1640625"/>
-    <col min="2" max="3" customWidth="true" style="2" width="59.6640625"/>
-    <col min="4" max="6" customWidth="true" style="2" width="23.6640625"/>
-    <col min="7" max="16384" style="2" width="8.83203125"/>
+    <col min="1" max="1" width="33.1328125" style="2" customWidth="1"/>
+    <col min="2" max="3" width="59.6640625" style="2" customWidth="1"/>
+    <col min="4" max="6" width="23.6640625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E4" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5" s="5" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -4830,7 +4965,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -4838,7 +4973,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -4846,7 +4981,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -4854,7 +4989,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -4862,7 +4997,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -4870,7 +5005,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -4878,7 +5013,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -4886,7 +5021,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -4894,7 +5029,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -4902,7 +5037,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -4910,7 +5045,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -4918,7 +5053,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -4926,7 +5061,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -4934,7 +5069,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -4942,7 +5077,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -4966,80 +5101,80 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="33.1640625"/>
-    <col min="2" max="3" customWidth="true" style="2" width="59.6640625"/>
-    <col min="4" max="7" customWidth="true" style="2" width="23.6640625"/>
-    <col min="8" max="16384" style="2" width="8.83203125"/>
+    <col min="1" max="1" width="33.1328125" style="2" customWidth="1"/>
+    <col min="2" max="3" width="59.6640625" style="2" customWidth="1"/>
+    <col min="4" max="7" width="23.6640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A2" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A4" s="9" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
-        <v>64</v>
-      </c>
       <c r="B4" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="G4" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" s="5" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6" s="5" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -5048,7 +5183,7 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -5057,7 +5192,7 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -5066,7 +5201,7 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -5075,7 +5210,7 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -5084,7 +5219,7 @@
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -5093,7 +5228,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -5102,7 +5237,7 @@
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -5111,7 +5246,7 @@
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -5120,7 +5255,7 @@
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -5129,7 +5264,7 @@
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -5138,7 +5273,7 @@
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -5147,7 +5282,7 @@
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -5156,7 +5291,7 @@
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -5165,7 +5300,7 @@
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -5190,156 +5325,156 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="33.1640625"/>
-    <col min="2" max="2" customWidth="true" style="2" width="59.6640625"/>
-    <col min="3" max="3" customWidth="true" style="2" width="39.33203125"/>
-    <col min="4" max="4" customWidth="true" style="2" width="32.83203125"/>
-    <col min="5" max="5" customWidth="true" style="2" width="34.6640625"/>
-    <col min="6" max="16384" style="2" width="8.83203125"/>
+    <col min="1" max="1" width="33.1328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="59.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="39.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="32.796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="34.6640625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A2" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A4" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -5360,36 +5495,36 @@
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="33.1640625"/>
-    <col min="2" max="2" customWidth="true" style="2" width="59.6640625"/>
-    <col min="3" max="3" customWidth="true" style="2" width="39.33203125"/>
-    <col min="4" max="5" customWidth="true" style="2" width="32.83203125"/>
-    <col min="6" max="6" customWidth="true" style="2" width="34.6640625"/>
-    <col min="7" max="16384" style="2" width="8.83203125"/>
+    <col min="1" max="1" width="33.1328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="59.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="39.33203125" style="2" customWidth="1"/>
+    <col min="4" max="5" width="32.796875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="34.6640625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A2" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A4" s="7" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>103</v>
-      </c>
       <c r="B4" s="26"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" s="9" t="s">
         <v>0</v>
       </c>
@@ -5397,35 +5532,35 @@
         <v>1</v>
       </c>
       <c r="C6" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="F6" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7" s="5" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -5433,7 +5568,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -5441,7 +5576,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -5449,7 +5584,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -5457,7 +5592,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -5465,7 +5600,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -5473,7 +5608,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -5481,7 +5616,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -5489,7 +5624,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -5497,7 +5632,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -5505,7 +5640,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -5513,7 +5648,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -5521,7 +5656,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -5529,7 +5664,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -5537,7 +5672,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -5545,7 +5680,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -5568,54 +5703,54 @@
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="6.1640625"/>
-    <col min="2" max="2" customWidth="true" style="2" width="33.1640625"/>
-    <col min="3" max="6" customWidth="true" style="2" width="36.1640625"/>
-    <col min="7" max="22" customWidth="true" style="2" width="15.0"/>
-    <col min="23" max="30" customWidth="true" style="2" width="32.83203125"/>
-    <col min="31" max="31" customWidth="true" style="2" width="34.6640625"/>
-    <col min="32" max="16384" style="2" width="8.83203125"/>
+    <col min="1" max="1" width="6.1328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.1328125" style="2" customWidth="1"/>
+    <col min="3" max="6" width="36.1328125" style="2" customWidth="1"/>
+    <col min="7" max="22" width="15" style="2" customWidth="1"/>
+    <col min="23" max="30" width="32.796875" style="2" customWidth="1"/>
+    <col min="31" max="31" width="34.6640625" style="2" customWidth="1"/>
+    <col min="32" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A2" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="4"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A4" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B2" s="4"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>110</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
@@ -5625,607 +5760,607 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="5" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A12" s="7"/>
       <c r="B12" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A13" s="7"/>
       <c r="B13" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A14" s="7"/>
       <c r="B14" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A15" s="7"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A16" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A17" s="7"/>
       <c r="B17" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A18" s="7"/>
       <c r="B18" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A19" s="7"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A20" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A21" s="7"/>
       <c r="B21" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A22" s="7"/>
       <c r="B22" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A23" s="7"/>
       <c r="B23" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A24" s="7"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A25" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A26" s="7"/>
       <c r="B26" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A27" s="7"/>
       <c r="B27" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A28" s="7"/>
       <c r="B28" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A29" s="7"/>
       <c r="B29" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A30" s="7"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A31" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A32" s="7"/>
       <c r="B32" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A33" s="7"/>
       <c r="B33" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A34" s="7"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A35" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A36" s="7"/>
       <c r="B36" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A37" s="7"/>
       <c r="B37" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A38" s="7"/>
       <c r="B38" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A39" s="7"/>
       <c r="B39" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A40" s="7"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A41" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A42" s="7"/>
       <c r="B42" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A43" s="7"/>
       <c r="B43" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A44" s="7"/>
       <c r="B44" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A45" s="7"/>
       <c r="B45" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A46" s="7"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A47" s="7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A48" s="7"/>
       <c r="B48" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A49" s="7"/>
       <c r="B49" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A50" s="7"/>
       <c r="B50" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A51" s="7"/>
       <c r="B51" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A52" s="7"/>
       <c r="B52" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A53" s="7"/>
       <c r="B53" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A54" s="7"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A55" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A56" s="7"/>
       <c r="B56" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A57" s="7"/>
       <c r="B57" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A58" s="7"/>
       <c r="B58" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A59" s="7"/>
       <c r="B59" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A60" s="7"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A61" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A62" s="7"/>
       <c r="B62" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A63" s="7"/>
       <c r="B63" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A64" s="7"/>
       <c r="B64" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A65" s="7"/>
       <c r="B65" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A66" s="7"/>
       <c r="B66" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A67" s="7"/>
       <c r="B67" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
       <c r="F67" s="5"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A68" s="7"/>
       <c r="B68" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A69" s="7"/>
       <c r="B69" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A70" s="7"/>
       <c r="B70" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A71" s="7"/>
       <c r="B71" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A72" s="7"/>
       <c r="B72" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A73" s="7"/>
       <c r="B73" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A74" s="7"/>
       <c r="B74" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A75" s="7"/>
       <c r="B75" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A76" s="7"/>
       <c r="B76" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A77" s="7"/>
       <c r="B77" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
       <c r="E77" s="5"/>
       <c r="F77" s="5"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A78" s="7"/>
       <c r="B78" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A79" s="7"/>
       <c r="B79" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A80" s="7"/>
       <c r="B80" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>

</xml_diff>